<commit_message>
updated plotting for figures
</commit_message>
<xml_diff>
--- a/doc/Supp/Total_kinetic_analysis_delta_I/Total_kinetic_analysis_interplay.xlsx
+++ b/doc/Supp/Total_kinetic_analysis_delta_I/Total_kinetic_analysis_interplay.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/37ce31b80bf1ee6d/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/37ce31b80bf1ee6d/Documents/r_projects/ptm_interplay_scoring/doc/Supp/Total_kinetic_analysis_delta_I/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="796" documentId="13_ncr:1_{724AD94A-F526-DE40-AC77-DFD0F6798C18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF62B2DC-3090-42EB-BD0F-3138C8158665}"/>
+  <xr:revisionPtr revIDLastSave="819" documentId="13_ncr:1_{724AD94A-F526-DE40-AC77-DFD0F6798C18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C369C24A-908C-4380-9FB7-4D220A034530}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2A2AF5B0-B513-45B3-A2BC-21C7C9F9A50E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{2A2AF5B0-B513-45B3-A2BC-21C7C9F9A50E}"/>
   </bookViews>
   <sheets>
-    <sheet name="interplay" sheetId="8" r:id="rId1"/>
-    <sheet name="interplay_calcs" sheetId="3" r:id="rId2"/>
-    <sheet name="discrete_PTM" sheetId="2" r:id="rId3"/>
-    <sheet name="og data " sheetId="7" r:id="rId4"/>
-    <sheet name="M4K" sheetId="9" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="10" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="11" r:id="rId2"/>
+    <sheet name="interplay" sheetId="8" r:id="rId3"/>
+    <sheet name="interplay_calcs" sheetId="3" r:id="rId4"/>
+    <sheet name="discrete_PTM" sheetId="2" r:id="rId5"/>
+    <sheet name="og data " sheetId="7" r:id="rId6"/>
+    <sheet name="M4K" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -70,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="108">
   <si>
     <t>K27un</t>
   </si>
@@ -426,6 +428,14 @@
   </si>
   <si>
     <t>K27 status</t>
+  </si>
+  <si>
+    <t>TKO PTM pair
+PTM2|PTM1</t>
+  </si>
+  <si>
+    <t>NTKO PTM pair
+PTM2|PTM1</t>
   </si>
 </sst>
 </file>
@@ -559,7 +569,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -604,6 +614,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,10 +643,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -948,11 +961,545 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19014C3F-D8FC-4F4A-98E8-67A6905FC745}">
+  <dimension ref="A1:B31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.90625" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6328125" style="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="20">
+        <v>-0.24132110512106303</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="20">
+        <v>-7.6209956412141927E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="20">
+        <v>0.1104350820045544</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="20">
+        <v>0.20709597952865078</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="20">
+        <v>-0.36929323739506742</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="20">
+        <v>-0.10259137598414933</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="20">
+        <v>0.38690755513843272</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="20">
+        <v>8.4977058240784206E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="20">
+        <v>0.4177175371077857</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="20">
+        <v>0.13417709864705712</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="20">
+        <v>-0.37135576885780519</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="20">
+        <v>-0.18053886689703763</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="20">
+        <v>0.33990013970093652</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="20">
+        <v>5.3301943740190746E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="20">
+        <v>-0.26874320898225273</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="20">
+        <v>-0.14712667759981307</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="20">
+        <v>-0.11833924537174283</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="20">
+        <v>8.9007635774966759E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="20">
+        <v>0.30933727979389253</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="20">
+        <v>-0.34112741450351702</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="20">
+        <v>-0.24136654978890446</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="20">
+        <v>0.47247252983396143</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="20">
+        <v>0.19231423528312735</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="20">
+        <v>0.39333439293343064</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="20">
+        <v>0.32179446551424506</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="20">
+        <v>-0.46226761982531778</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="20">
+        <v>-0.41649941737262097</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="20">
+        <v>9.4919699169899632E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="20">
+        <v>3.7911329646402162E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="20">
+        <v>-9.9212545783610037E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21692095-0689-4F0D-9A40-51EA73CA6A8E}">
+  <dimension ref="A1:B31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="A1" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2">
+        <v>8.6632332381368637E-5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3">
+        <v>-2.4460190949609842E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4">
+        <v>-9.6825074384313203E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5">
+        <v>0.12119863300154145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6">
+        <v>-7.4495687676660288E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7">
+        <v>-0.14458483318435483</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8">
+        <v>0.28428961418597376</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9">
+        <v>-6.5209093324958375E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10">
+        <v>0.1740033470802701</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11">
+        <v>0.47193084693084691</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12">
+        <v>-0.55546590161974785</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13">
+        <v>-9.0468292391369304E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14">
+        <v>0.50415828303152244</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15">
+        <v>0.32655935613682091</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16">
+        <v>-0.73212608987256877</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17">
+        <v>4.5368501744341705E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18">
+        <v>-5.8204668884528937E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19">
+        <v>-9.8539779826889773E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20">
+        <v>0.22910337350214022</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21">
+        <v>-0.48240797234085814</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22">
+        <v>-0.42543148795814495</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23">
+        <v>0.35776154297510393</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24">
+        <v>-0.15242311645189355</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25">
+        <v>0.36435600193989459</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26">
+        <v>0.44902470926099697</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27">
+        <v>-0.22603466464795707</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28">
+        <v>-6.837920558372769E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29">
+        <v>0.11759828538352031</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30">
+        <v>3.461144758167705E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31">
+        <v>-3.318709850025691E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43F8C56A-7184-4259-91E7-E57670DFE741}">
   <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A16"/>
+    <sheetView topLeftCell="E1" zoomScale="87" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1815,10 +2362,11 @@
     <mergeCell ref="J1:J16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0EC4700-B312-467D-910C-80016B2F08B9}">
   <dimension ref="A1:AG30"/>
   <sheetViews>
@@ -3796,7 +4344,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BDF6649-0E36-4FCC-9766-71B51A48EBD1}">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -3913,7 +4461,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D23F6BE-9A48-6A49-AC8A-BCC1C22E358F}">
   <dimension ref="A1:C16"/>
   <sheetViews>
@@ -4107,7 +4655,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BBD11A0-D83F-452C-BDF0-0F381F674E12}">
   <dimension ref="A1:AK11"/>
   <sheetViews>

</xml_diff>